<commit_message>
updated forecasting model + data
</commit_message>
<xml_diff>
--- a/Data/Forecasting/quarterly_beer_reports.xlsx
+++ b/Data/Forecasting/quarterly_beer_reports.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,10 +498,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>43466</v>
+        <v>42370</v>
       </c>
       <c r="C6" t="n">
-        <v>141770.84</v>
+        <v>144673.26</v>
       </c>
     </row>
     <row r="7">
@@ -509,10 +509,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>43556</v>
+        <v>42461</v>
       </c>
       <c r="C7" t="n">
-        <v>174361.65</v>
+        <v>164690.01</v>
       </c>
     </row>
     <row r="8">
@@ -520,10 +520,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>43647</v>
+        <v>42552</v>
       </c>
       <c r="C8" t="n">
-        <v>172197.77</v>
+        <v>159577.78</v>
       </c>
     </row>
     <row r="9">
@@ -531,10 +531,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>43739</v>
+        <v>42644</v>
       </c>
       <c r="C9" t="n">
-        <v>152382.04</v>
+        <v>130911.14</v>
       </c>
     </row>
     <row r="10">
@@ -542,10 +542,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>43831</v>
+        <v>42736</v>
       </c>
       <c r="C10" t="n">
-        <v>143716.36</v>
+        <v>129666.67</v>
       </c>
     </row>
     <row r="11">
@@ -553,10 +553,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>43922</v>
+        <v>42826</v>
       </c>
       <c r="C11" t="n">
-        <v>134249.77</v>
+        <v>154792.88</v>
       </c>
     </row>
     <row r="12">
@@ -564,10 +564,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44013</v>
+        <v>42917</v>
       </c>
       <c r="C12" t="n">
-        <v>177946.83</v>
+        <v>151173.56</v>
       </c>
     </row>
     <row r="13">
@@ -575,10 +575,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44105</v>
+        <v>43009</v>
       </c>
       <c r="C13" t="n">
-        <v>119758</v>
+        <v>129257.67</v>
       </c>
     </row>
     <row r="14">
@@ -586,10 +586,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44197</v>
+        <v>43101</v>
       </c>
       <c r="C14" t="n">
-        <v>135495.88</v>
+        <v>138059.06</v>
       </c>
     </row>
     <row r="15">
@@ -597,10 +597,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44287</v>
+        <v>43191</v>
       </c>
       <c r="C15" t="n">
-        <v>178675.73</v>
+        <v>151559.7</v>
       </c>
     </row>
     <row r="16">
@@ -608,10 +608,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44378</v>
+        <v>43282</v>
       </c>
       <c r="C16" t="n">
-        <v>190195.37</v>
+        <v>176406.12</v>
       </c>
     </row>
     <row r="17">
@@ -619,10 +619,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44470</v>
+        <v>43374</v>
       </c>
       <c r="C17" t="n">
-        <v>144776.51</v>
+        <v>141318.62</v>
       </c>
     </row>
     <row r="18">
@@ -630,10 +630,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44562</v>
+        <v>43466</v>
       </c>
       <c r="C18" t="n">
-        <v>143975.2300000001</v>
+        <v>141770.84</v>
       </c>
     </row>
     <row r="19">
@@ -641,10 +641,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44652</v>
+        <v>43556</v>
       </c>
       <c r="C19" t="n">
-        <v>178701.3259999999</v>
+        <v>174361.65</v>
       </c>
     </row>
     <row r="20">
@@ -652,10 +652,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44743</v>
+        <v>43647</v>
       </c>
       <c r="C20" t="n">
-        <v>173138.676</v>
+        <v>172197.77</v>
       </c>
     </row>
     <row r="21">
@@ -663,10 +663,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44835</v>
+        <v>43739</v>
       </c>
       <c r="C21" t="n">
-        <v>142074.2400000001</v>
+        <v>152382.04</v>
       </c>
     </row>
     <row r="22">
@@ -674,10 +674,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44927</v>
+        <v>43831</v>
       </c>
       <c r="C22" t="n">
-        <v>142340.79</v>
+        <v>143716.36</v>
       </c>
     </row>
     <row r="23">
@@ -685,10 +685,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45017</v>
+        <v>43922</v>
       </c>
       <c r="C23" t="n">
-        <v>161582.11</v>
+        <v>134249.77</v>
       </c>
     </row>
     <row r="24">
@@ -696,9 +696,141 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="n">
+        <v>44013</v>
+      </c>
+      <c r="C24" t="n">
+        <v>177946.83</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>44105</v>
+      </c>
+      <c r="C25" t="n">
+        <v>119758</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>44197</v>
+      </c>
+      <c r="C26" t="n">
+        <v>135495.88</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>44287</v>
+      </c>
+      <c r="C27" t="n">
+        <v>178675.73</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>44378</v>
+      </c>
+      <c r="C28" t="n">
+        <v>190195.37</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>44470</v>
+      </c>
+      <c r="C29" t="n">
+        <v>144776.51</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>44562</v>
+      </c>
+      <c r="C30" t="n">
+        <v>143975.2300000001</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>44652</v>
+      </c>
+      <c r="C31" t="n">
+        <v>178701.3259999999</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>44743</v>
+      </c>
+      <c r="C32" t="n">
+        <v>173138.676</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>44835</v>
+      </c>
+      <c r="C33" t="n">
+        <v>142074.2400000001</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>44927</v>
+      </c>
+      <c r="C34" t="n">
+        <v>142340.79</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>45017</v>
+      </c>
+      <c r="C35" t="n">
+        <v>161582.11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="n">
         <v>45108</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C36" t="n">
         <v>156378.82</v>
       </c>
     </row>

</xml_diff>